<commit_message>
docs : add excel file
메일링 대상자들에 대한 이름,이메일 주소가 담긴 엑셀 파일 추가
</commit_message>
<xml_diff>
--- a/3week/email_list.xlsx
+++ b/3week/email_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\유영미\Documents\dev\KDT_HW\3week\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF5D310-0FD2-4322-A43C-690CC8F3BA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4703AF2B-FB46-4080-8381-039755544BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="612" windowWidth="7644" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="612" windowWidth="17040" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -142,11 +142,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -457,25 +457,25 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="5">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4"/>

</xml_diff>